<commit_message>
battle 6 difficulty tuning
</commit_message>
<xml_diff>
--- a/contents/battle/battle_6/battle_6.xlsx
+++ b/contents/battle/battle_6/battle_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle\battle_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625AE1A9-16D3-4A08-9D5B-EAFAB1D3CB6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAE1E46-4305-4EF9-8C55-EC33C561C632}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="58">
   <si>
     <t>x</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>forest</t>
+  </si>
+  <si>
+    <t>walls</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,6 +281,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -291,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -306,6 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,10 +654,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>49</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -661,10 +674,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>49</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -678,10 +694,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>49</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -712,10 +731,13 @@
         <v>4</v>
       </c>
       <c r="D6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>49</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -729,10 +751,13 @@
         <v>5</v>
       </c>
       <c r="D7" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>49</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -780,10 +805,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>49</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -797,10 +825,13 @@
         <v>6</v>
       </c>
       <c r="D11" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>49</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -848,10 +879,13 @@
         <v>6</v>
       </c>
       <c r="D14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>49</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -865,10 +899,13 @@
         <v>7</v>
       </c>
       <c r="D15" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>49</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -888,7 +925,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -905,7 +942,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -922,7 +959,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -933,13 +970,16 @@
         <v>7</v>
       </c>
       <c r="D19" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -950,13 +990,16 @@
         <v>8</v>
       </c>
       <c r="D20" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -973,7 +1016,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -990,7 +1033,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1007,7 +1050,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1018,13 +1061,16 @@
         <v>8</v>
       </c>
       <c r="D24" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1035,13 +1081,16 @@
         <v>9</v>
       </c>
       <c r="D25" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1058,7 +1107,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1075,7 +1124,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1092,7 +1141,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1103,13 +1152,16 @@
         <v>9</v>
       </c>
       <c r="D29" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1120,13 +1172,16 @@
         <v>10</v>
       </c>
       <c r="D30" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1143,7 +1198,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1160,7 +1215,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1177,7 +1232,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1188,13 +1243,16 @@
         <v>10</v>
       </c>
       <c r="D34" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1205,13 +1263,16 @@
         <v>11</v>
       </c>
       <c r="D35" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1228,7 +1289,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1245,7 +1306,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1256,13 +1317,16 @@
         <v>11</v>
       </c>
       <c r="D38" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1273,13 +1337,16 @@
         <v>12</v>
       </c>
       <c r="D39" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1296,7 +1363,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1307,13 +1374,16 @@
         <v>12</v>
       </c>
       <c r="D41" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1324,13 +1394,16 @@
         <v>13</v>
       </c>
       <c r="D42" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1341,13 +1414,16 @@
         <v>13</v>
       </c>
       <c r="D43" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1364,7 +1440,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
@@ -1381,7 +1457,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
@@ -1398,7 +1474,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
@@ -1415,7 +1491,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>
@@ -2729,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE17DB7-E6BE-4178-A86C-3E370AE7D84E}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,7 +3228,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I12" s="2">
         <v>101</v>
@@ -3187,7 +3263,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I13" s="2">
         <v>102</v>
@@ -3222,7 +3298,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I14" s="2">
         <v>103</v>
@@ -3257,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I15" s="2">
         <v>104</v>
@@ -3274,31 +3350,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="8">
-        <v>4</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>46</v>
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="8">
-        <v>2</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>0</v>
-      </c>
-      <c r="H16" s="8">
-        <v>6</v>
-      </c>
-      <c r="I16" s="2">
-        <v>105</v>
+        <v>45</v>
+      </c>
+      <c r="E16" s="5">
+        <v>3</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2</v>
+      </c>
+      <c r="H16" s="5">
+        <v>7</v>
+      </c>
+      <c r="I16" s="1">
+        <v>94</v>
       </c>
       <c r="J16" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K16" s="8">
         <v>3</v>
@@ -3327,10 +3403,10 @@
         <v>2</v>
       </c>
       <c r="H17" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I17" s="1">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J17" s="8">
         <v>1</v>
@@ -3362,10 +3438,10 @@
         <v>2</v>
       </c>
       <c r="H18" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I18" s="1">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J18" s="8">
         <v>1</v>
@@ -3397,10 +3473,10 @@
         <v>2</v>
       </c>
       <c r="H19" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I19" s="1">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J19" s="8">
         <v>1</v>
@@ -3416,32 +3492,32 @@
       <c r="B20" s="8">
         <v>1</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="5">
-        <v>3</v>
-      </c>
-      <c r="F20" s="5">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5">
-        <v>2</v>
-      </c>
-      <c r="H20" s="5">
-        <v>6</v>
-      </c>
-      <c r="I20" s="1">
-        <v>97</v>
+      <c r="C20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20" s="13">
+        <v>3</v>
       </c>
       <c r="J20" s="8">
         <v>1</v>
       </c>
       <c r="K20" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3470,13 +3546,13 @@
         <v>5</v>
       </c>
       <c r="I21" s="13">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="J21" s="8">
         <v>1</v>
       </c>
       <c r="K21" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3505,7 +3581,7 @@
         <v>5</v>
       </c>
       <c r="I22" s="13">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J22" s="8">
         <v>1</v>
@@ -3715,7 +3791,7 @@
         <v>5</v>
       </c>
       <c r="I28" s="13">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="J28" s="8">
         <v>1</v>
@@ -3750,16 +3826,16 @@
         <v>5</v>
       </c>
       <c r="I29" s="13">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="J29" s="8">
         <v>1</v>
       </c>
       <c r="K29" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -3785,27 +3861,49 @@
         <v>5</v>
       </c>
       <c r="I30" s="13">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="J30" s="8">
         <v>1</v>
       </c>
       <c r="K30" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
+      <c r="A31" s="8">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31" s="13">
+        <v>2</v>
+      </c>
+      <c r="J31" s="8">
+        <v>1</v>
+      </c>
+      <c r="K31" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
@@ -3819,6 +3917,19 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
difficulty tuning, knights feel more powerful in comparison
</commit_message>
<xml_diff>
--- a/contents/battle/battle_6/battle_6.xlsx
+++ b/contents/battle/battle_6/battle_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle\battle_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820CEC28-9831-4EA9-864C-B08F3E0E853D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125C8701-22D6-4FBA-9E58-AE7475FE8658}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="58">
   <si>
     <t>x</t>
   </si>
@@ -2805,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE17DB7-E6BE-4178-A86C-3E370AE7D84E}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2878,7 +2878,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I2" s="9">
         <v>43</v>
@@ -2913,7 +2913,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I3" s="9">
         <v>48</v>
@@ -2948,7 +2948,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4" s="9">
         <v>51</v>
@@ -2983,7 +2983,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I5" s="9">
         <v>54</v>
@@ -3018,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6" s="9">
         <v>56</v>
@@ -3053,7 +3053,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I7" s="9">
         <v>59</v>
@@ -3088,7 +3088,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8" s="9">
         <v>62</v>
@@ -3123,7 +3123,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I9" s="9">
         <v>65</v>
@@ -3158,7 +3158,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I10" s="9">
         <v>68</v>
@@ -3193,7 +3193,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I11" s="9">
         <v>72</v>
@@ -3212,11 +3212,11 @@
       <c r="B12" s="8">
         <v>4</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>46</v>
+      <c r="C12" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="E12" s="8">
         <v>2</v>
@@ -3225,16 +3225,16 @@
         <v>0</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="8">
         <v>5</v>
       </c>
-      <c r="I12" s="2">
-        <v>101</v>
+      <c r="I12" s="9">
+        <v>76</v>
       </c>
       <c r="J12" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K12" s="8">
         <v>3</v>
@@ -3263,10 +3263,10 @@
         <v>0</v>
       </c>
       <c r="H13" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I13" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J13" s="8">
         <v>1</v>
@@ -3298,10 +3298,10 @@
         <v>0</v>
       </c>
       <c r="H14" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I14" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J14" s="8">
         <v>1</v>
@@ -3333,13 +3333,13 @@
         <v>0</v>
       </c>
       <c r="H15" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I15" s="2">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J15" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K15" s="8">
         <v>3</v>
@@ -3350,34 +3350,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="8">
-        <v>1</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>47</v>
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="5">
-        <v>3</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5">
-        <v>2</v>
-      </c>
-      <c r="H16" s="5">
-        <v>7</v>
-      </c>
-      <c r="I16" s="13">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="E16" s="8">
+        <v>2</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
+        <v>4</v>
+      </c>
+      <c r="I16" s="2">
+        <v>104</v>
       </c>
       <c r="J16" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3385,34 +3385,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="8">
-        <v>1</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>47</v>
+        <v>4</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="5">
-        <v>3</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5">
-        <v>2</v>
-      </c>
-      <c r="H17" s="5">
-        <v>7</v>
-      </c>
-      <c r="I17" s="13">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="E17" s="8">
+        <v>2</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
+        <v>4</v>
+      </c>
+      <c r="I17" s="2">
+        <v>105</v>
       </c>
       <c r="J17" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K17" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3441,13 +3441,13 @@
         <v>7</v>
       </c>
       <c r="I18" s="13">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J18" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3476,13 +3476,13 @@
         <v>7</v>
       </c>
       <c r="I19" s="13">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J19" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3492,32 +3492,32 @@
       <c r="B20" s="8">
         <v>1</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>5</v>
+      <c r="C20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="5">
+        <v>3</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>2</v>
+      </c>
+      <c r="H20" s="5">
+        <v>7</v>
       </c>
       <c r="I20" s="13">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="J20" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3527,32 +3527,32 @@
       <c r="B21" s="8">
         <v>1</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>5</v>
+      <c r="C21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="5">
+        <v>3</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <v>2</v>
+      </c>
+      <c r="H21" s="5">
+        <v>7</v>
       </c>
       <c r="I21" s="13">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="J21" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3581,13 +3581,13 @@
         <v>5</v>
       </c>
       <c r="I22" s="13">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="J22" s="8">
         <v>1</v>
       </c>
       <c r="K22" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3616,7 +3616,7 @@
         <v>5</v>
       </c>
       <c r="I23" s="13">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="J23" s="8">
         <v>1</v>
@@ -3651,13 +3651,13 @@
         <v>5</v>
       </c>
       <c r="I24" s="13">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J24" s="8">
         <v>1</v>
       </c>
       <c r="K24" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3686,13 +3686,13 @@
         <v>5</v>
       </c>
       <c r="I25" s="13">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="J25" s="8">
         <v>1</v>
       </c>
       <c r="K25" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3702,17 +3702,17 @@
       <c r="B26" s="8">
         <v>1</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>48</v>
+      <c r="C26" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E26">
         <v>2</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -3721,13 +3721,13 @@
         <v>5</v>
       </c>
       <c r="I26" s="13">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="J26" s="8">
         <v>1</v>
       </c>
       <c r="K26" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3737,17 +3737,17 @@
       <c r="B27" s="8">
         <v>1</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>48</v>
+      <c r="C27" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -3756,13 +3756,13 @@
         <v>5</v>
       </c>
       <c r="I27" s="13">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="J27" s="8">
         <v>1</v>
       </c>
       <c r="K27" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3791,7 +3791,7 @@
         <v>5</v>
       </c>
       <c r="I28" s="13">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="J28" s="8">
         <v>1</v>
@@ -3826,7 +3826,7 @@
         <v>5</v>
       </c>
       <c r="I29" s="13">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="J29" s="8">
         <v>1</v>
@@ -3861,16 +3861,16 @@
         <v>5</v>
       </c>
       <c r="I30" s="13">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="J30" s="8">
         <v>1</v>
       </c>
       <c r="K30" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -3896,48 +3896,48 @@
         <v>5</v>
       </c>
       <c r="I31" s="13">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="J31" s="8">
         <v>1</v>
       </c>
       <c r="K31" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>31</v>
       </c>
       <c r="B32" s="8">
         <v>1</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="5">
-        <v>3</v>
-      </c>
-      <c r="F32" s="5">
-        <v>0</v>
-      </c>
-      <c r="G32" s="5">
-        <v>2</v>
-      </c>
-      <c r="H32" s="5">
-        <v>7</v>
-      </c>
-      <c r="I32" s="1">
-        <v>94</v>
+      <c r="C32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="I32" s="13">
+        <v>23</v>
       </c>
       <c r="J32" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K32" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -3947,32 +3947,32 @@
       <c r="B33" s="8">
         <v>1</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="5">
-        <v>3</v>
-      </c>
-      <c r="F33" s="5">
-        <v>0</v>
-      </c>
-      <c r="G33" s="5">
-        <v>2</v>
-      </c>
-      <c r="H33" s="5">
-        <v>7</v>
-      </c>
-      <c r="I33" s="1">
-        <v>95</v>
+      <c r="C33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+      <c r="I33" s="13">
+        <v>2</v>
       </c>
       <c r="J33" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K33" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -4001,7 +4001,7 @@
         <v>7</v>
       </c>
       <c r="I34" s="1">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J34" s="8">
         <v>3</v>
@@ -4036,12 +4036,82 @@
         <v>7</v>
       </c>
       <c r="I35" s="1">
+        <v>95</v>
+      </c>
+      <c r="J35" s="8">
+        <v>1</v>
+      </c>
+      <c r="K35" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>35</v>
+      </c>
+      <c r="B36" s="8">
+        <v>1</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="5">
+        <v>3</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0</v>
+      </c>
+      <c r="G36" s="5">
+        <v>2</v>
+      </c>
+      <c r="H36" s="5">
+        <v>7</v>
+      </c>
+      <c r="I36" s="1">
+        <v>96</v>
+      </c>
+      <c r="J36" s="8">
+        <v>1</v>
+      </c>
+      <c r="K36" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>36</v>
+      </c>
+      <c r="B37" s="8">
+        <v>1</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="5">
+        <v>3</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <v>2</v>
+      </c>
+      <c r="H37" s="5">
+        <v>7</v>
+      </c>
+      <c r="I37" s="1">
         <v>97</v>
       </c>
-      <c r="J35" s="8">
-        <v>3</v>
-      </c>
-      <c r="K35" s="8">
+      <c r="J37" s="8">
+        <v>1</v>
+      </c>
+      <c r="K37" s="8">
         <v>3</v>
       </c>
     </row>

</xml_diff>